<commit_message>
Output Excel sheet updated
</commit_message>
<xml_diff>
--- a/Project/Output of Dataset with variable HTM Parameters (version 1).xlsb.xlsx
+++ b/Project/Output of Dataset with variable HTM Parameters (version 1).xlsb.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aiman\source\repos\neocortexapi-classification\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aiman\source\repos\Image-classification\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED512D9A-56BC-41F1-9478-1623F44355C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDEBDBFE-8F63-4133-B935-90A31B4B474E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="97">
   <si>
     <t>S.No</t>
   </si>
@@ -311,6 +310,12 @@
   </si>
   <si>
     <t>https://github.com/Alam-Sher-Khan/neocortexapi-classification/blob/Aiman/Project/Test%20Exp%2036/Output.JPG</t>
+  </si>
+  <si>
+    <t>Test Exp 37</t>
+  </si>
+  <si>
+    <t>https://github.com/Alam-Sher-Khan/neocortexapi-classification/blob/Aiman/Project/Test%20Exp%2037/Prediction%20output%20with%20correct%20result%20for%20test%20images%20different%20from%20input%20images.JPG</t>
   </si>
 </sst>
 </file>
@@ -356,7 +361,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -379,12 +384,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -403,8 +419,14 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -687,10 +709,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O37"/>
+  <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O46" sqref="O46"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -735,11 +757,11 @@
       <c r="H1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
       <c r="L1" s="7" t="s">
         <v>85</v>
       </c>
@@ -2444,6 +2466,56 @@
       <c r="O37" s="8" t="s">
         <v>94</v>
       </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A38" s="4">
+        <v>37</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C38" s="10">
+        <v>1</v>
+      </c>
+      <c r="D38" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F38" s="4">
+        <v>-1</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I38" s="4">
+        <v>65.08</v>
+      </c>
+      <c r="J38" s="2">
+        <v>57.39</v>
+      </c>
+      <c r="K38" s="2">
+        <v>44.81</v>
+      </c>
+      <c r="L38" s="2">
+        <v>51.16</v>
+      </c>
+      <c r="M38" s="2">
+        <v>65.319999999999993</v>
+      </c>
+      <c r="N38" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="O38" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A39" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2485,8 +2557,9 @@
     <hyperlink ref="O35" r:id="rId33" xr:uid="{BF895A59-815D-4720-9993-4C35D6ECF714}"/>
     <hyperlink ref="O36" r:id="rId34" xr:uid="{A0230EDF-92FD-4456-8020-85DAF78B993C}"/>
     <hyperlink ref="O37" r:id="rId35" xr:uid="{E50763B7-C8DC-4AF6-B0E2-B954234840D5}"/>
+    <hyperlink ref="O38" r:id="rId36" xr:uid="{312ED256-DCB8-46EF-9ABE-8E8E023B5044}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId36"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId37"/>
 </worksheet>
 </file>
</xml_diff>